<commit_message>
ssh only pc 22
</commit_message>
<xml_diff>
--- a/checkMatrix.xlsx
+++ b/checkMatrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Desktop\netzwerk_projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Desktop\netzwerk_projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BA004B-5746-4EC1-B798-4648889A60FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138D3282-A610-4D39-9AF9-7C3CFCF3CA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{BA46FD15-E9EB-456C-9B97-D37AF1513905}"/>
+    <workbookView xWindow="20850" yWindow="0" windowWidth="17655" windowHeight="20985" xr2:uid="{BA46FD15-E9EB-456C-9B97-D37AF1513905}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="18">
-  <si>
-    <t>PC1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="17">
   <si>
     <t>WEB-Server</t>
   </si>
@@ -45,9 +42,6 @@
     <t>80,443,ping</t>
   </si>
   <si>
-    <t>Border-Router</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -60,25 +54,28 @@
     <t>x(nat)</t>
   </si>
   <si>
-    <t>x(telnet,ssh,snmp)</t>
-  </si>
-  <si>
-    <t>y(telnet,ssh,snmp)</t>
-  </si>
-  <si>
-    <t>PC3</t>
-  </si>
-  <si>
-    <t>Server_DNS/IOT</t>
-  </si>
-  <si>
-    <t>google.com</t>
-  </si>
-  <si>
-    <t>Laptop0</t>
-  </si>
-  <si>
-    <t>y(ip)</t>
+    <t>PC11</t>
+  </si>
+  <si>
+    <t>PC21</t>
+  </si>
+  <si>
+    <t>DNS/IOT-Server</t>
+  </si>
+  <si>
+    <t>PC22</t>
+  </si>
+  <si>
+    <t>ISP-Router</t>
+  </si>
+  <si>
+    <t>x(ssh)</t>
+  </si>
+  <si>
+    <t>y(ssh)</t>
+  </si>
+  <si>
+    <t>x(80,443)</t>
   </si>
 </sst>
 </file>
@@ -124,7 +121,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -140,9 +137,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -180,7 +177,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -286,7 +283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,275 +433,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA4D826-5D93-4107-88B0-FCE5926A56B6}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated acls on isp to only allow pc22 and iot devices to reach dns/iot-server
</commit_message>
<xml_diff>
--- a/checkMatrix.xlsx
+++ b/checkMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tobias\Desktop\netzwerk_projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EB9BB8-E408-466B-A164-38F7A4D91BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE6C797-7FB2-4224-8F93-59E9E9110E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{BA46FD15-E9EB-456C-9B97-D37AF1513905}"/>
+    <workbookView xWindow="10320" yWindow="4320" windowWidth="28800" windowHeight="15345" xr2:uid="{BA46FD15-E9EB-456C-9B97-D37AF1513905}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="18">
   <si>
     <t>WEB-Server</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>IoT-Laptop</t>
+  </si>
+  <si>
+    <t>y(80,443)</t>
   </si>
 </sst>
 </file>
@@ -436,14 +439,13 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -466,10 +468,10 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -495,10 +497,10 @@
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -524,10 +526,10 @@
         <v>3</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -553,10 +555,10 @@
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -570,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
@@ -582,10 +584,10 @@
         <v>4</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -599,7 +601,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
@@ -611,56 +613,56 @@
         <v>5</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>3</v>
@@ -669,10 +671,10 @@
         <v>3</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>